<commit_message>
finished everythion i think for cs457 programming assignment
</commit_message>
<xml_diff>
--- a/Senior Yr/Fall/cs457/ProgrammingAssignment1/analysis/dataSheet.xlsx
+++ b/Senior Yr/Fall/cs457/ProgrammingAssignment1/analysis/dataSheet.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sunny\Classwork\Senior Yr\Fall\cs457\ProgrammingAssignment1\analysis\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="13020" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Heapsort" sheetId="1" r:id="rId1"/>
@@ -24,8 +19,11 @@
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -82,7 +80,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +99,22 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,68 +135,80 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -211,7 +237,19 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -272,7 +310,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -281,26 +318,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -370,25 +387,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -457,25 +474,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -544,25 +561,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -591,12 +608,13 @@
             <a:effectLst/>
           </c:spPr>
         </c:hiLowLines>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="131344800"/>
-        <c:axId val="131348720"/>
+        <c:axId val="1845512536"/>
+        <c:axId val="1845504856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="131344800"/>
+        <c:axId val="1845512536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,7 +646,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -637,26 +654,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -695,7 +692,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131348720"/>
+        <c:crossAx val="1845504856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -703,7 +700,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131348720"/>
+        <c:axId val="1845504856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -753,8 +750,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.5000000000000001E-2"/>
-              <c:y val="0.38499234470691163"/>
+              <c:x val="0.025"/>
+              <c:y val="0.384992344706912"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -765,26 +762,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
@@ -817,7 +794,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131344800"/>
+        <c:crossAx val="1845512536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -831,7 +808,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -940,25 +916,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1K</c:v>
+                  <c:v>_x0002_1K</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5K</c:v>
+                  <c:v>_x0002_5K</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10K</c:v>
+                  <c:v>_x0003_10K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15K</c:v>
+                  <c:v>_x0003_15K</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20K</c:v>
+                  <c:v>_x0003_20K</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25K</c:v>
+                  <c:v>_x0003_25K</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50K</c:v>
+                  <c:v>_x0003_50K</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -970,25 +946,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1015,25 +991,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1K</c:v>
+                  <c:v>_x0002_1K</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5K</c:v>
+                  <c:v>_x0002_5K</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10K</c:v>
+                  <c:v>_x0003_10K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15K</c:v>
+                  <c:v>_x0003_15K</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20K</c:v>
+                  <c:v>_x0003_20K</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25K</c:v>
+                  <c:v>_x0003_25K</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50K</c:v>
+                  <c:v>_x0003_50K</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1045,25 +1021,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1090,25 +1066,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1K</c:v>
+                  <c:v>_x0002_1K</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5K</c:v>
+                  <c:v>_x0002_5K</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10K</c:v>
+                  <c:v>_x0003_10K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15K</c:v>
+                  <c:v>_x0003_15K</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20K</c:v>
+                  <c:v>_x0003_20K</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25K</c:v>
+                  <c:v>_x0003_25K</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50K</c:v>
+                  <c:v>_x0003_50K</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1120,25 +1096,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1153,11 +1129,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="131352640"/>
-        <c:axId val="35157872"/>
+        <c:axId val="1848161512"/>
+        <c:axId val="1848167272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="131352640"/>
+        <c:axId val="1848161512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1184,14 +1160,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="35157872"/>
+        <c:crossAx val="1848167272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1199,7 +1174,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35157872"/>
+        <c:axId val="1848167272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1222,21 +1197,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131352640"/>
+        <c:crossAx val="1848161512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1245,7 +1218,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1281,7 +1254,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1312,25 +1284,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1K</c:v>
+                  <c:v>_x0002_1K</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5K</c:v>
+                  <c:v>_x0002_5K</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10K</c:v>
+                  <c:v>_x0003_10K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15K</c:v>
+                  <c:v>_x0003_15K</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20K</c:v>
+                  <c:v>_x0003_20K</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25K</c:v>
+                  <c:v>_x0003_25K</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50K</c:v>
+                  <c:v>_x0003_50K</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1342,25 +1314,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1387,25 +1359,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1K</c:v>
+                  <c:v>_x0002_1K</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5K</c:v>
+                  <c:v>_x0002_5K</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10K</c:v>
+                  <c:v>_x0003_10K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15K</c:v>
+                  <c:v>_x0003_15K</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20K</c:v>
+                  <c:v>_x0003_20K</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25K</c:v>
+                  <c:v>_x0003_25K</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50K</c:v>
+                  <c:v>_x0003_50K</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1417,25 +1389,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1462,25 +1434,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1K</c:v>
+                  <c:v>_x0002_1K</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5K</c:v>
+                  <c:v>_x0002_5K</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10K</c:v>
+                  <c:v>_x0003_10K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15K</c:v>
+                  <c:v>_x0003_15K</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20K</c:v>
+                  <c:v>_x0003_20K</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25K</c:v>
+                  <c:v>_x0003_25K</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50K</c:v>
+                  <c:v>_x0003_50K</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1492,25 +1464,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1525,11 +1497,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="184982912"/>
-        <c:axId val="184983472"/>
+        <c:axId val="1848202264"/>
+        <c:axId val="1848207768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="184982912"/>
+        <c:axId val="1848202264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1551,14 +1523,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184983472"/>
+        <c:crossAx val="1848207768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1566,7 +1537,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="184983472"/>
+        <c:axId val="1848207768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,21 +1560,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184982912"/>
+        <c:crossAx val="1848202264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1612,7 +1581,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1633,6 +1602,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparing</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> sorting algorithms </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1642,26 +1641,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1731,25 +1710,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1818,25 +1797,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1905,25 +1884,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1992,25 +1971,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2025,18 +2004,44 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="235509232"/>
-        <c:axId val="235510912"/>
+        <c:axId val="1848267752"/>
+        <c:axId val="1847205656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="235509232"/>
+        <c:axId val="1848267752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size of input</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -2046,26 +2051,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2104,7 +2089,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235510912"/>
+        <c:crossAx val="1847205656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2112,7 +2097,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235510912"/>
+        <c:axId val="1847205656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2133,6 +2118,36 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Milliseconds</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Elapsed</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -2142,26 +2157,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2194,7 +2189,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235509232"/>
+        <c:crossAx val="1848267752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2275,1103 +2270,917 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparing sorting algorithms</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Random!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insertion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Random!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Random!$B$2:$H$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>529.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>949.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1539.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5853.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Random!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mergesort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Random!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Random!$B$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Random!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quicksort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Random!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Random!$B$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Random!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Heapsort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Random!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Random!$B$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1849493496"/>
+        <c:axId val="1826809544"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1849493496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size of input</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1826809544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1826809544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Milliseconds</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> elapsed</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1849493496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sorting algorithms compared</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reverse!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insertion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Reverse!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reverse!$B$2:$H$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>467.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1076.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1895.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2924.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11715.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reverse!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mergesort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Reverse!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reverse!$B$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reverse!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quicksort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Reverse!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reverse!$B$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reverse!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Heapsort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Reverse!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reverse!$B$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1849406440"/>
+        <c:axId val="1849415640"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1849406440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size of input</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1849415640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1849415640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Milliseconds  elcapsed</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1849406440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3518,8 +3327,78 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -3634,7 +3513,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -3791,7 +3670,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3826,7 +3705,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4003,7 +3882,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4017,9 +3896,9 @@
       <selection activeCell="H3" sqref="B3:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="16" thickBot="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4042,7 +3921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="16" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -4068,7 +3947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="16" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -4094,7 +3973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -4122,8 +4001,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4135,12 +4018,12 @@
       <selection activeCell="B4" sqref="B4:H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="16" thickBot="1">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -4164,7 +4047,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="16" thickBot="1">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -4190,7 +4073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="16" thickBot="1">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -4216,7 +4099,7 @@
         <v>5853</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16" thickBot="1">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -4244,6 +4127,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4255,9 +4143,9 @@
       <selection activeCell="B4" sqref="B4:H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4280,7 +4168,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -4306,7 +4194,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4332,7 +4220,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4361,6 +4249,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4372,12 +4265,12 @@
       <selection activeCell="B4" sqref="B4:H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4400,7 +4293,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -4426,7 +4319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4452,7 +4345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4481,6 +4374,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4488,16 +4386,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4520,7 +4418,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -4546,7 +4444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -4572,7 +4470,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -4598,7 +4496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="17.25" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -4626,7 +4524,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4635,15 +4539,15 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H4"/>
+      <selection activeCell="H5" sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="16" thickBot="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4666,7 +4570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="16" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -4692,7 +4596,7 @@
         <v>5853</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="16" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -4718,7 +4622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -4744,7 +4648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -4772,6 +4676,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4779,16 +4690,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4811,7 +4722,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -4837,7 +4748,7 @@
         <v>11715</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="21" customHeight="1" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -4863,7 +4774,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="21" customHeight="1" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -4889,7 +4800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="21" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -4917,5 +4828,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>